<commit_message>
Truven 2022 Q2 finalized and pub to DW
</commit_message>
<xml_diff>
--- a/greenplum/datawarehouse/QA/truven/dw_staging/outputs/02-truven-raw-counts.xlsx
+++ b/greenplum/datawarehouse/QA/truven/dw_staging/outputs/02-truven-raw-counts.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t xml:space="preserve">Count of distinct claim IDs (msclmid) in Truven schema on TACC server</t>
   </si>
   <si>
-    <t xml:space="preserve">Run time: 2023-01-13 12:02:05</t>
+    <t xml:space="preserve">Run time: 2023-05-15 21:54:41</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -135,48 +135,57 @@
     <t xml:space="preserve">12651429</t>
   </si>
   <si>
-    <t xml:space="preserve">6912682</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43887419</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1966294</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13362344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6885963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46324960</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3091594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17636955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6512965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43595978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3265064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16446722</t>
+    <t xml:space="preserve">7116117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46581035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4040704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24373789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6955080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47443203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3965780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21212781</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7042238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50122078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3365903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17657731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3092203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26477138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1608515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9207855</t>
   </si>
   <si>
     <t xml:space="preserve">Count of distinct enrolid-msclmid combinations in Truven schema on TACC server</t>
   </si>
   <si>
-    <t xml:space="preserve">Run time: 2023-01-13 12:02:06</t>
-  </si>
-  <si>
     <t xml:space="preserve">truv_concat_ccaes</t>
   </si>
   <si>
@@ -285,40 +294,52 @@
     <t xml:space="preserve">26105481</t>
   </si>
   <si>
-    <t xml:space="preserve">10100319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">236770305</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2272431</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25794549</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9462462</t>
-  </si>
-  <si>
-    <t xml:space="preserve">216097356</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3361488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31580107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9098129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">226696842</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3571308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34270777</t>
+    <t xml:space="preserve">10313174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">242648514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4434376</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42280008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9529231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">217834210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4322960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39967388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9698020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240648715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3646460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34798051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4020059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108987165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1722930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17597041</t>
   </si>
   <si>
     <t xml:space="preserve">Count of distinct enrolid-msclmid combinations in Truven schema on TACC server (rows with dx codes only, enrolid DOES NOT have to exist in 'a' tables)</t>
@@ -339,127 +360,43 @@
     <t xml:space="preserve">22342428</t>
   </si>
   <si>
-    <t xml:space="preserve">464918374</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10836651</t>
-  </si>
-  <si>
-    <t xml:space="preserve">106388169</t>
-  </si>
-  <si>
     <t xml:space="preserve">21969947</t>
   </si>
   <si>
-    <t xml:space="preserve">474856537</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10014362</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99229449</t>
-  </si>
-  <si>
     <t xml:space="preserve">16810938</t>
   </si>
   <si>
-    <t xml:space="preserve">373623657</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8711786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87971413</t>
-  </si>
-  <si>
     <t xml:space="preserve">17911818</t>
   </si>
   <si>
-    <t xml:space="preserve">398987590</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7964782</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79453231</t>
-  </si>
-  <si>
     <t xml:space="preserve">11500592</t>
   </si>
   <si>
-    <t xml:space="preserve">253980315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5184304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49680954</t>
-  </si>
-  <si>
     <t xml:space="preserve">11596396</t>
   </si>
   <si>
-    <t xml:space="preserve">262995594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4812826</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48794435</t>
-  </si>
-  <si>
     <t xml:space="preserve">10576642</t>
   </si>
   <si>
-    <t xml:space="preserve">244020676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34051690</t>
-  </si>
-  <si>
     <t xml:space="preserve">10976665</t>
   </si>
   <si>
-    <t xml:space="preserve">250109632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26060687</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10100175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">235614972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25752925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9462360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">214867927</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31508576</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9098102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">225833663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3571306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34009715</t>
+    <t xml:space="preserve">10312481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9528771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9697992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4020050</t>
   </si>
   <si>
     <t xml:space="preserve">Count of distinct enrolid-msclmid combinations in Truven schema on TACC server (rows with proc codes only, counting from 's' and 'f' tables)</t>
   </si>
   <si>
-    <t xml:space="preserve">Run time: 2023-01-13 12:02:07</t>
+    <t xml:space="preserve">Run time: 2023-05-15 21:54:42</t>
   </si>
   <si>
     <t xml:space="preserve">truv_proc_ccae</t>
@@ -516,22 +453,28 @@
     <t xml:space="preserve">1607341</t>
   </si>
   <si>
-    <t xml:space="preserve">7615794</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1592479</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7192444</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2471845</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7097762</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2310381</t>
+    <t xml:space="preserve">7762081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3010790</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7234219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2964896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7558410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2357368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3059756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1055642</t>
   </si>
   <si>
     <t xml:space="preserve">Note that ccaes/ccaef tables were combined, then count distinct (otherwise there are too many overlaps)</t>
@@ -594,22 +537,28 @@
     <t xml:space="preserve">29537128</t>
   </si>
   <si>
-    <t xml:space="preserve">189840924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25335171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">175061759</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33544584</t>
-  </si>
-  <si>
-    <t xml:space="preserve">169771182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33684593</t>
+    <t xml:space="preserve">194924194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42628776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">176884613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43155669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">178636852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34030942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79778481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16754551</t>
   </si>
 </sst>
 </file>
@@ -1155,6 +1104,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -1171,12 +1137,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1184,16 +1150,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
@@ -1201,16 +1167,16 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -1218,16 +1184,16 @@
         <v>2012</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -1235,16 +1201,16 @@
         <v>2013</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -1252,16 +1218,16 @@
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -1269,16 +1235,16 @@
         <v>2015</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
@@ -1286,16 +1252,16 @@
         <v>2016</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11">
@@ -1303,16 +1269,16 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
@@ -1320,16 +1286,16 @@
         <v>2018</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13">
@@ -1337,16 +1303,16 @@
         <v>2019</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
@@ -1354,16 +1320,16 @@
         <v>2020</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
@@ -1371,16 +1337,33 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1399,12 +1382,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1412,16 +1395,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
@@ -1429,187 +1412,132 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" t="s">
-        <v>109</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>2012</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>113</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>2013</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" t="s">
         <v>115</v>
       </c>
-      <c r="D7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" t="s">
-        <v>117</v>
-      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" t="s">
-        <v>121</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>2015</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" t="s">
-        <v>125</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>2016</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" t="s">
-        <v>129</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s">
-        <v>132</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>2018</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" t="s">
-        <v>135</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>2019</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" t="s">
-        <v>138</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>2020</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" t="s">
-        <v>141</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" t="s">
-        <v>145</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1627,12 +1555,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
@@ -1640,10 +1568,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5">
@@ -1651,10 +1579,10 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6">
@@ -1662,10 +1590,10 @@
         <v>2012</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
@@ -1673,10 +1601,10 @@
         <v>2013</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8">
@@ -1684,10 +1612,10 @@
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9">
@@ -1695,10 +1623,10 @@
         <v>2015</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10">
@@ -1706,10 +1634,10 @@
         <v>2016</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11">
@@ -1717,10 +1645,10 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12">
@@ -1728,10 +1656,10 @@
         <v>2018</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13">
@@ -1739,10 +1667,10 @@
         <v>2019</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14">
@@ -1750,10 +1678,10 @@
         <v>2020</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15">
@@ -1761,15 +1689,26 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>172</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1788,12 +1727,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
@@ -1801,10 +1740,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
@@ -1812,10 +1751,10 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
@@ -1823,10 +1762,10 @@
         <v>2012</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
@@ -1834,10 +1773,10 @@
         <v>2013</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
@@ -1845,10 +1784,10 @@
         <v>2014</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9">
@@ -1856,10 +1795,10 @@
         <v>2015</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10">
@@ -1867,10 +1806,10 @@
         <v>2016</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
@@ -1878,10 +1817,10 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
@@ -1889,10 +1828,10 @@
         <v>2018</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
@@ -1900,10 +1839,10 @@
         <v>2019</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14">
@@ -1911,10 +1850,10 @@
         <v>2020</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15">
@@ -1922,10 +1861,21 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>